<commit_message>
Subida dia 09 Marzo
</commit_message>
<xml_diff>
--- a/mi_archivo.xlsx
+++ b/mi_archivo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas_2\Desktop\Django 04032023\Django_horarios_V6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35934A4-4B05-4959-ADA4-051A4C573FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315ECF00-E519-4A4A-872F-FF958F806882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -506,12 +506,12 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Cambios en home al ingresar, cambios en el texto y estilo en los botones de exportar e importar excel
</commit_message>
<xml_diff>
--- a/mi_archivo.xlsx
+++ b/mi_archivo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas_2\Desktop\Django 04032023\Django_horarios_V6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas.HEAVENSFRUIT\Documents\HeavensDev\Horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315ECF00-E519-4A4A-872F-FF958F806882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A41393-786E-44EC-A5CA-88DF01934DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>ftt</t>
+  </si>
+  <si>
+    <t>nicolas</t>
   </si>
 </sst>
 </file>
@@ -503,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517EB25E-5F15-4935-8D9C-647B88A2BAF3}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -582,7 +585,7 @@
         <v>44987</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -614,7 +617,7 @@
         <v>44987</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -646,7 +649,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -678,7 +681,7 @@
         <v>44985</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -710,7 +713,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -742,7 +745,7 @@
         <v>44978</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -774,7 +777,7 @@
         <v>44979</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -806,7 +809,7 @@
         <v>44980</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -838,7 +841,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -870,7 +873,7 @@
         <v>44982</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -902,7 +905,7 @@
         <v>44983</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -934,7 +937,7 @@
         <v>44984</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18</v>
       </c>
@@ -966,7 +969,7 @@
         <v>44985</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>19</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>44987</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>21</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>44988</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>22</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>44989</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>23</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>24</v>
       </c>
@@ -1155,6 +1158,38 @@
         <v>22</v>
       </c>
       <c r="J20" s="1">
+        <v>44991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>4354653</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3100000</v>
+      </c>
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="1">
         <v>44991</v>
       </c>
     </row>

</xml_diff>